<commit_message>
Perubahan pada kelebihan jam mengajar sekarang tidak ada di tabel transport namun ada di tabel pegawai dan disable edit password pada admin karene error terus, DBnya baru OK
</commit_message>
<xml_diff>
--- a/asset/file/DATA GUKAR.xlsx
+++ b/asset/file/DATA GUKAR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\penggajian\asset\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B4C75CA-F347-4E9E-BE5C-801E01333230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F644EF5A-245E-4F53-9ED9-78CFBB340FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4BEF8F3C-ADBD-431E-8EB6-DE1979333483}"/>
+    <workbookView xWindow="4590" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{4BEF8F3C-ADBD-431E-8EB6-DE1979333483}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="161">
   <si>
     <t>DATA GUKAR</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Kelebihan Jam</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -621,18 +624,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -676,6 +689,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -992,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52E8D34-81B6-4154-BA9C-D1262C0A6A15}">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,24 +1031,26 @@
     <col min="9" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1062,15 +1084,18 @@
       <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="L2" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
         <v>1141955</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1091,18 +1116,19 @@
       <c r="I3" s="1">
         <v>89212121</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="K3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>331006</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1123,18 +1149,19 @@
       <c r="I4" s="1">
         <v>89212121</v>
       </c>
-      <c r="K4" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="K4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>1275881</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1155,18 +1182,19 @@
       <c r="I5" s="1">
         <v>89212121</v>
       </c>
-      <c r="K5" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="K5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>1422682</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1190,18 +1218,19 @@
       <c r="J6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="K6" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="K6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
         <v>989256</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>145</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1222,18 +1251,19 @@
       <c r="I7" s="1">
         <v>89212121</v>
       </c>
-      <c r="K7" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="K7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>1275882</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1254,18 +1284,19 @@
       <c r="I8" s="1">
         <v>89212121</v>
       </c>
-      <c r="K8" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="K8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>1141959</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1286,18 +1317,19 @@
       <c r="I9" s="1">
         <v>89212121</v>
       </c>
-      <c r="K9" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="K9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>331010</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1318,18 +1350,19 @@
       <c r="I10" s="1">
         <v>89212121</v>
       </c>
-      <c r="K10" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="K10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>331008</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1350,18 +1383,19 @@
       <c r="I11" s="1">
         <v>89212121</v>
       </c>
-      <c r="K11" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="K11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>331005</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1382,18 +1416,19 @@
       <c r="I12" s="1">
         <v>89212121</v>
       </c>
-      <c r="K12" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="K12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>821110</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1414,18 +1449,19 @@
       <c r="I13" s="1">
         <v>89212121</v>
       </c>
-      <c r="K13" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="K13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>359177</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1446,18 +1482,19 @@
       <c r="I14" s="1">
         <v>89212121</v>
       </c>
-      <c r="K14" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="K14" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
         <v>221004</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1478,18 +1515,19 @@
       <c r="I15" s="1">
         <v>89212121</v>
       </c>
-      <c r="K15" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="K15" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>989251</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1510,18 +1548,19 @@
       <c r="I16" s="1">
         <v>89212121</v>
       </c>
-      <c r="K16" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="K16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
         <v>1426551</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1542,18 +1581,19 @@
       <c r="I17" s="1">
         <v>89212121</v>
       </c>
-      <c r="K17" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="K17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <v>1122231</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>111</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1574,18 +1614,19 @@
       <c r="I18" s="1">
         <v>89212121</v>
       </c>
-      <c r="K18" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="K18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>1065555</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1606,18 +1647,19 @@
       <c r="I19" s="1">
         <v>89212121</v>
       </c>
-      <c r="K19" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="K19" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
         <v>1024573</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>79</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1638,18 +1680,19 @@
       <c r="I20" s="1">
         <v>89212121</v>
       </c>
-      <c r="K20" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="K20" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>1040717</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1670,18 +1713,19 @@
       <c r="I21" s="1">
         <v>89212121</v>
       </c>
-      <c r="K21" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="K21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
         <v>221002</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1702,18 +1746,19 @@
       <c r="I22" s="1">
         <v>89212121</v>
       </c>
-      <c r="K22" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="K22" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>1231479</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1734,18 +1779,19 @@
       <c r="I23" s="1">
         <v>89212121</v>
       </c>
-      <c r="K23" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="K23" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
         <v>3412323</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1766,18 +1812,19 @@
       <c r="I24" s="1">
         <v>89212121</v>
       </c>
-      <c r="K24" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="K24" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
         <v>938403</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>83</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1798,18 +1845,19 @@
       <c r="I25" s="1">
         <v>89212121</v>
       </c>
-      <c r="K25" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="K25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>1141962</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1830,18 +1878,19 @@
       <c r="I26" s="1">
         <v>89212121</v>
       </c>
-      <c r="K26" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="K26" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>1141957</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1862,18 +1911,19 @@
       <c r="I27" s="1">
         <v>89212121</v>
       </c>
-      <c r="K27" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="K27" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>1034902</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1894,18 +1944,19 @@
       <c r="I28" s="1">
         <v>89212121</v>
       </c>
-      <c r="K28" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="K28" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>1065558</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1926,18 +1977,19 @@
       <c r="I29" s="1">
         <v>89212121</v>
       </c>
-      <c r="K29" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="K29" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
         <v>1141960</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1958,18 +2010,19 @@
       <c r="I30" s="1">
         <v>89212121</v>
       </c>
-      <c r="K30" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="K30" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
         <v>3333333</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1990,18 +2043,19 @@
       <c r="I31" s="1">
         <v>89212121</v>
       </c>
-      <c r="K31" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="K31" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="18">
         <v>221005</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>127</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2022,18 +2076,19 @@
       <c r="I32" s="1">
         <v>89212121</v>
       </c>
-      <c r="K32" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="K32" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
         <v>1141952</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -2054,18 +2109,19 @@
       <c r="I33" s="1">
         <v>89212121</v>
       </c>
-      <c r="K33" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="K33" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="10">
         <v>331011</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>88</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2086,18 +2142,19 @@
       <c r="I34" s="1">
         <v>89212121</v>
       </c>
-      <c r="K34" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+      <c r="K34" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
         <v>1425699</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -2118,18 +2175,19 @@
       <c r="I35" s="1">
         <v>89212121</v>
       </c>
-      <c r="K35" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="K35" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>989247</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -2150,18 +2208,19 @@
       <c r="I36" s="1">
         <v>89212121</v>
       </c>
-      <c r="K36" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="K36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
         <v>1165561</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -2182,18 +2241,19 @@
       <c r="I37" s="1">
         <v>89212121</v>
       </c>
-      <c r="K37" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="K37" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
         <v>11111111</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>113</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2214,18 +2274,19 @@
       <c r="I38" s="1">
         <v>89212121</v>
       </c>
-      <c r="K38" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="K38" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>221003</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2246,18 +2307,19 @@
       <c r="I39" s="1">
         <v>89212121</v>
       </c>
-      <c r="K39" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="K39" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
         <v>1141950</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -2278,18 +2340,19 @@
       <c r="I40" s="1">
         <v>89212121</v>
       </c>
-      <c r="K40" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="19">
+      <c r="K40" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="18">
         <v>221006</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>129</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2310,18 +2373,19 @@
       <c r="I41" s="1">
         <v>89212121</v>
       </c>
-      <c r="K41" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="K41" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>938410</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2342,18 +2406,19 @@
       <c r="I42" s="1">
         <v>89212121</v>
       </c>
-      <c r="K42" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+      <c r="K42" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
         <v>221008</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>149</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2374,18 +2439,19 @@
       <c r="I43" s="1">
         <v>89212121</v>
       </c>
-      <c r="K43" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
+      <c r="K43" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="19">
         <v>2132334</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>138</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2406,18 +2472,19 @@
       <c r="I44" s="1">
         <v>89212121</v>
       </c>
-      <c r="K44" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
+      <c r="K44" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="14">
         <v>938408</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>131</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2438,18 +2505,19 @@
       <c r="I45" s="1">
         <v>89212121</v>
       </c>
-      <c r="K45" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
+      <c r="K45" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="14">
         <v>1048519</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2470,18 +2538,19 @@
       <c r="I46" s="1">
         <v>89212121</v>
       </c>
-      <c r="K46" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="K46" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="10">
         <v>1065563</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>79</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2502,18 +2571,19 @@
       <c r="I47" s="1">
         <v>89212121</v>
       </c>
-      <c r="K47" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
+      <c r="K47" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="14">
         <v>1231332</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="15" t="s">
         <v>153</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -2534,18 +2604,19 @@
       <c r="I48" s="1">
         <v>89212121</v>
       </c>
-      <c r="K48" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="K48" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="10">
         <v>1078964</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D49" s="1" t="s">
@@ -2566,18 +2637,19 @@
       <c r="I49" s="1">
         <v>89212121</v>
       </c>
-      <c r="K49" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="K49" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
         <v>1141965</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -2598,18 +2670,19 @@
       <c r="I50" s="1">
         <v>89212121</v>
       </c>
-      <c r="K50" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
+      <c r="K50" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
         <v>1335504</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2630,18 +2703,19 @@
       <c r="I51" s="1">
         <v>89212121</v>
       </c>
-      <c r="K51" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="15">
+      <c r="K51" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
         <v>221001</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>134</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -2662,18 +2736,19 @@
       <c r="I52" s="1">
         <v>89212121</v>
       </c>
-      <c r="K52" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
+      <c r="K52" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="10">
         <v>938396</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2694,18 +2769,19 @@
       <c r="I53" s="1">
         <v>89212121</v>
       </c>
-      <c r="K53" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="K53" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
         <v>1102147</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2726,18 +2802,19 @@
       <c r="I54" s="1">
         <v>89212121</v>
       </c>
-      <c r="K54" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="19">
+      <c r="K54" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="18">
         <v>221007</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="9" t="s">
         <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2758,18 +2835,19 @@
       <c r="I55" s="1">
         <v>89212121</v>
       </c>
-      <c r="K55" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="K55" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
         <v>1141963</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -2790,18 +2868,19 @@
       <c r="I56" s="1">
         <v>89212121</v>
       </c>
-      <c r="K56" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="11">
+      <c r="K56" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L56" s="1"/>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="10">
         <v>938398</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -2822,18 +2901,19 @@
       <c r="I57" s="1">
         <v>89212121</v>
       </c>
-      <c r="K57" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="K57" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="8">
         <v>1312155</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -2854,18 +2934,19 @@
       <c r="I58" s="1">
         <v>89212121</v>
       </c>
-      <c r="K58" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="15">
+      <c r="K58" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" s="1"/>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
         <v>1141947</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>123</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -2886,18 +2967,19 @@
       <c r="I59" s="1">
         <v>89212121</v>
       </c>
-      <c r="K59" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="K59" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L59" s="1"/>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
         <v>1266023</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2918,18 +3000,19 @@
       <c r="I60" s="1">
         <v>89212121</v>
       </c>
-      <c r="K60" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="K60" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L60" s="1"/>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
         <v>838656</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2950,18 +3033,19 @@
       <c r="I61" s="1">
         <v>89212121</v>
       </c>
-      <c r="K61" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="19">
+      <c r="K61" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="18">
         <v>221009</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>138</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2982,18 +3066,19 @@
       <c r="I62" s="1">
         <v>89212121</v>
       </c>
-      <c r="K62" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="11">
+      <c r="K62" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A63" s="10">
         <v>938391</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>99</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3014,18 +3099,19 @@
       <c r="I63" s="1">
         <v>89212121</v>
       </c>
-      <c r="K63" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="15">
+      <c r="K63" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
         <v>938401</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>140</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -3046,18 +3132,19 @@
       <c r="I64" s="1">
         <v>89212121</v>
       </c>
-      <c r="K64" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="11">
+      <c r="K64" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A65" s="10">
         <v>1141964</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3078,18 +3165,19 @@
       <c r="I65" s="1">
         <v>89212121</v>
       </c>
-      <c r="K65" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="K65" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L65" s="1"/>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
         <v>1188171</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -3110,18 +3198,19 @@
       <c r="I66" s="1">
         <v>89212121</v>
       </c>
-      <c r="K66" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="K66" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L66" s="1"/>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="8">
         <v>331004</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>103</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3142,18 +3231,19 @@
       <c r="I67" s="1">
         <v>89212121</v>
       </c>
-      <c r="K67" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="11">
+      <c r="K67" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L67" s="1"/>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A68" s="10">
         <v>989245</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -3174,18 +3264,19 @@
       <c r="I68" s="1">
         <v>89212121</v>
       </c>
-      <c r="K68" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="K68" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L68" s="1"/>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
         <v>1188172</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3206,18 +3297,19 @@
       <c r="I69" s="1">
         <v>89212121</v>
       </c>
-      <c r="K69" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="15">
+      <c r="K69" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L69" s="1"/>
+    </row>
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="14">
         <v>4231212</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="9" t="s">
         <v>119</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -3238,18 +3330,19 @@
       <c r="I70" s="1">
         <v>89212121</v>
       </c>
-      <c r="K70" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="15">
+      <c r="K70" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L70" s="1"/>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="14">
         <v>938402</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3270,18 +3363,19 @@
       <c r="I71" s="1">
         <v>89212121</v>
       </c>
-      <c r="K71" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="K71" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L71" s="1"/>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
         <v>989254</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -3302,18 +3396,19 @@
       <c r="I72" s="1">
         <v>89212121</v>
       </c>
-      <c r="K72" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="K72" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L72" s="1"/>
+    </row>
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
         <v>1024572</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3334,18 +3429,19 @@
       <c r="I73" s="1">
         <v>89212121</v>
       </c>
-      <c r="K73" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="K73" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L73" s="1"/>
+    </row>
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
         <v>331001</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -3366,18 +3462,19 @@
       <c r="I74" s="1">
         <v>89212121</v>
       </c>
-      <c r="K74" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="K74" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L74" s="1"/>
+    </row>
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
         <v>1034905</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3398,18 +3495,19 @@
       <c r="I75" s="1">
         <v>89212121</v>
       </c>
-      <c r="K75" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="15">
+      <c r="K75" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L75" s="1"/>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A76" s="14">
         <v>938395</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="9" t="s">
         <v>140</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -3430,18 +3528,19 @@
       <c r="I76" s="1">
         <v>89212121</v>
       </c>
-      <c r="K76" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+      <c r="K76" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L76" s="1"/>
+    </row>
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A77" s="8">
         <v>331007</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3462,18 +3561,19 @@
       <c r="I77" s="1">
         <v>89212121</v>
       </c>
-      <c r="K77" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="15">
+      <c r="K77" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A78" s="14">
         <v>1336410</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B78" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="15" t="s">
         <v>115</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -3494,18 +3594,19 @@
       <c r="I78" s="1">
         <v>89212121</v>
       </c>
-      <c r="K78" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="17">
+      <c r="K78" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L78" s="1"/>
+    </row>
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="16">
         <v>938406</v>
       </c>
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="17" t="s">
         <v>121</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3526,18 +3627,19 @@
       <c r="I79" s="1">
         <v>89212121</v>
       </c>
-      <c r="K79" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="12">
+      <c r="K79" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L79" s="1"/>
+    </row>
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A80" s="11">
         <v>1099552</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="12" t="s">
         <v>68</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -3558,18 +3660,19 @@
       <c r="I80" s="1">
         <v>89212121</v>
       </c>
-      <c r="K80" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="K80" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L80" s="1"/>
+    </row>
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
         <v>1191276</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3590,18 +3693,19 @@
       <c r="I81" s="1">
         <v>89212121</v>
       </c>
-      <c r="K81" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="20">
+      <c r="K81" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L81" s="1"/>
+    </row>
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A82" s="19">
         <v>221011</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="C82" s="15" t="s">
         <v>151</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -3622,18 +3726,19 @@
       <c r="I82" s="1">
         <v>89212121</v>
       </c>
-      <c r="K82" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="K82" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L82" s="1"/>
+    </row>
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
         <v>1136922</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3654,18 +3759,19 @@
       <c r="I83" s="1">
         <v>89212121</v>
       </c>
-      <c r="K83" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="11">
+      <c r="K83" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L83" s="1"/>
+    </row>
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A84" s="10">
         <v>1065554</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="9" t="s">
         <v>109</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -3686,18 +3792,19 @@
       <c r="I84" s="1">
         <v>89212121</v>
       </c>
-      <c r="K84" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="19">
+      <c r="K84" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L84" s="1"/>
+    </row>
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A85" s="18">
         <v>221010</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B85" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C85" s="9" t="s">
         <v>138</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -3718,16 +3825,30 @@
       <c r="I85" s="1">
         <v>89212121</v>
       </c>
-      <c r="K85" s="21" t="s">
-        <v>12</v>
-      </c>
+      <c r="K85" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L85" s="1"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="22"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
+      <c r="J86" s="22"/>
+      <c r="K86" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K85">
     <sortCondition ref="B3:B85"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Menambahkan sweetaler 2 dan penambahan tmt serta penambahan tunjangan pangan, namun tmt masih menunggu tabel
</commit_message>
<xml_diff>
--- a/asset/file/DATA GUKAR.xlsx
+++ b/asset/file/DATA GUKAR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\penggajian\asset\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F644EF5A-245E-4F53-9ED9-78CFBB340FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E5A83E-780D-4D56-A481-969EBB8462FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{4BEF8F3C-ADBD-431E-8EB6-DE1979333483}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4BEF8F3C-ADBD-431E-8EB6-DE1979333483}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="162">
   <si>
     <t>DATA GUKAR</t>
   </si>
@@ -513,10 +513,13 @@
     <t>Wonosobo</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Kelebihan Jam</t>
+  </si>
+  <si>
+    <t>Guru Ekstra</t>
+  </si>
+  <si>
+    <t>Bukan Wali Kelas</t>
   </si>
 </sst>
 </file>
@@ -689,11 +692,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1015,7 +1018,7 @@
   <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,30 +1028,30 @@
     <col min="3" max="3" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1084,8 +1087,8 @@
       <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>160</v>
+      <c r="L2" s="22" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1102,7 +1105,7 @@
         <v>155</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>156</v>
@@ -1115,6 +1118,9 @@
       </c>
       <c r="I3" s="1">
         <v>89212121</v>
+      </c>
+      <c r="J3" s="1">
+        <v>4</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>12</v>
@@ -1149,6 +1155,9 @@
       <c r="I4" s="1">
         <v>89212121</v>
       </c>
+      <c r="J4" s="1">
+        <v>4</v>
+      </c>
       <c r="K4" s="20" t="s">
         <v>12</v>
       </c>
@@ -1182,6 +1191,9 @@
       <c r="I5" s="1">
         <v>89212121</v>
       </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
       <c r="K5" s="20" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1216,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>157</v>
@@ -1215,8 +1227,8 @@
       <c r="I6" s="1">
         <v>89212121</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>159</v>
+      <c r="J6" s="1">
+        <v>1</v>
       </c>
       <c r="K6" s="20" t="s">
         <v>12</v>
@@ -1251,6 +1263,9 @@
       <c r="I7" s="1">
         <v>89212121</v>
       </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
       <c r="K7" s="20" t="s">
         <v>12</v>
       </c>
@@ -1284,6 +1299,9 @@
       <c r="I8" s="1">
         <v>89212121</v>
       </c>
+      <c r="J8" s="1">
+        <v>4</v>
+      </c>
       <c r="K8" s="20" t="s">
         <v>12</v>
       </c>
@@ -1317,6 +1335,9 @@
       <c r="I9" s="1">
         <v>89212121</v>
       </c>
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
       <c r="K9" s="20" t="s">
         <v>12</v>
       </c>
@@ -1350,6 +1371,9 @@
       <c r="I10" s="1">
         <v>89212121</v>
       </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
       <c r="K10" s="20" t="s">
         <v>12</v>
       </c>
@@ -1383,6 +1407,9 @@
       <c r="I11" s="1">
         <v>89212121</v>
       </c>
+      <c r="J11" s="1">
+        <v>4</v>
+      </c>
       <c r="K11" s="20" t="s">
         <v>12</v>
       </c>
@@ -1416,6 +1443,9 @@
       <c r="I12" s="1">
         <v>89212121</v>
       </c>
+      <c r="J12" s="1">
+        <v>4</v>
+      </c>
       <c r="K12" s="20" t="s">
         <v>12</v>
       </c>
@@ -1449,6 +1479,9 @@
       <c r="I13" s="1">
         <v>89212121</v>
       </c>
+      <c r="J13" s="1">
+        <v>4</v>
+      </c>
       <c r="K13" s="20" t="s">
         <v>12</v>
       </c>
@@ -1482,6 +1515,9 @@
       <c r="I14" s="1">
         <v>89212121</v>
       </c>
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
       <c r="K14" s="20" t="s">
         <v>12</v>
       </c>
@@ -1515,6 +1551,9 @@
       <c r="I15" s="1">
         <v>89212121</v>
       </c>
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
       <c r="K15" s="20" t="s">
         <v>12</v>
       </c>
@@ -1548,6 +1587,9 @@
       <c r="I16" s="1">
         <v>89212121</v>
       </c>
+      <c r="J16" s="1">
+        <v>4</v>
+      </c>
       <c r="K16" s="20" t="s">
         <v>12</v>
       </c>
@@ -1581,6 +1623,9 @@
       <c r="I17" s="1">
         <v>89212121</v>
       </c>
+      <c r="J17" s="1">
+        <v>4</v>
+      </c>
       <c r="K17" s="20" t="s">
         <v>12</v>
       </c>
@@ -1614,6 +1659,9 @@
       <c r="I18" s="1">
         <v>89212121</v>
       </c>
+      <c r="J18" s="1">
+        <v>4</v>
+      </c>
       <c r="K18" s="20" t="s">
         <v>12</v>
       </c>
@@ -1647,6 +1695,9 @@
       <c r="I19" s="1">
         <v>89212121</v>
       </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
       <c r="K19" s="20" t="s">
         <v>12</v>
       </c>
@@ -1680,6 +1731,9 @@
       <c r="I20" s="1">
         <v>89212121</v>
       </c>
+      <c r="J20" s="1">
+        <v>4</v>
+      </c>
       <c r="K20" s="20" t="s">
         <v>12</v>
       </c>
@@ -1713,6 +1767,9 @@
       <c r="I21" s="1">
         <v>89212121</v>
       </c>
+      <c r="J21" s="1">
+        <v>4</v>
+      </c>
       <c r="K21" s="20" t="s">
         <v>12</v>
       </c>
@@ -1746,6 +1803,9 @@
       <c r="I22" s="1">
         <v>89212121</v>
       </c>
+      <c r="J22" s="1">
+        <v>4</v>
+      </c>
       <c r="K22" s="20" t="s">
         <v>12</v>
       </c>
@@ -1779,6 +1839,9 @@
       <c r="I23" s="1">
         <v>89212121</v>
       </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
       <c r="K23" s="20" t="s">
         <v>12</v>
       </c>
@@ -1812,6 +1875,9 @@
       <c r="I24" s="1">
         <v>89212121</v>
       </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
       <c r="K24" s="20" t="s">
         <v>12</v>
       </c>
@@ -1845,6 +1911,9 @@
       <c r="I25" s="1">
         <v>89212121</v>
       </c>
+      <c r="J25" s="1">
+        <v>4</v>
+      </c>
       <c r="K25" s="20" t="s">
         <v>12</v>
       </c>
@@ -1878,6 +1947,9 @@
       <c r="I26" s="1">
         <v>89212121</v>
       </c>
+      <c r="J26" s="1">
+        <v>4</v>
+      </c>
       <c r="K26" s="20" t="s">
         <v>12</v>
       </c>
@@ -1911,6 +1983,9 @@
       <c r="I27" s="1">
         <v>89212121</v>
       </c>
+      <c r="J27" s="1">
+        <v>4</v>
+      </c>
       <c r="K27" s="20" t="s">
         <v>12</v>
       </c>
@@ -1944,6 +2019,9 @@
       <c r="I28" s="1">
         <v>89212121</v>
       </c>
+      <c r="J28" s="1">
+        <v>4</v>
+      </c>
       <c r="K28" s="20" t="s">
         <v>12</v>
       </c>
@@ -1977,6 +2055,9 @@
       <c r="I29" s="1">
         <v>89212121</v>
       </c>
+      <c r="J29" s="1">
+        <v>4</v>
+      </c>
       <c r="K29" s="20" t="s">
         <v>12</v>
       </c>
@@ -2010,6 +2091,9 @@
       <c r="I30" s="1">
         <v>89212121</v>
       </c>
+      <c r="J30" s="1">
+        <v>4</v>
+      </c>
       <c r="K30" s="20" t="s">
         <v>12</v>
       </c>
@@ -2043,6 +2127,9 @@
       <c r="I31" s="1">
         <v>89212121</v>
       </c>
+      <c r="J31" s="1">
+        <v>4</v>
+      </c>
       <c r="K31" s="20" t="s">
         <v>12</v>
       </c>
@@ -2076,6 +2163,9 @@
       <c r="I32" s="1">
         <v>89212121</v>
       </c>
+      <c r="J32" s="1">
+        <v>4</v>
+      </c>
       <c r="K32" s="20" t="s">
         <v>12</v>
       </c>
@@ -2109,6 +2199,9 @@
       <c r="I33" s="1">
         <v>89212121</v>
       </c>
+      <c r="J33" s="1">
+        <v>4</v>
+      </c>
       <c r="K33" s="20" t="s">
         <v>12</v>
       </c>
@@ -2142,6 +2235,9 @@
       <c r="I34" s="1">
         <v>89212121</v>
       </c>
+      <c r="J34" s="1">
+        <v>4</v>
+      </c>
       <c r="K34" s="20" t="s">
         <v>12</v>
       </c>
@@ -2175,6 +2271,9 @@
       <c r="I35" s="1">
         <v>89212121</v>
       </c>
+      <c r="J35" s="1">
+        <v>4</v>
+      </c>
       <c r="K35" s="20" t="s">
         <v>12</v>
       </c>
@@ -2208,6 +2307,9 @@
       <c r="I36" s="1">
         <v>89212121</v>
       </c>
+      <c r="J36" s="1">
+        <v>4</v>
+      </c>
       <c r="K36" s="20" t="s">
         <v>12</v>
       </c>
@@ -2241,6 +2343,9 @@
       <c r="I37" s="1">
         <v>89212121</v>
       </c>
+      <c r="J37" s="1">
+        <v>4</v>
+      </c>
       <c r="K37" s="20" t="s">
         <v>12</v>
       </c>
@@ -2274,6 +2379,9 @@
       <c r="I38" s="1">
         <v>89212121</v>
       </c>
+      <c r="J38" s="1">
+        <v>4</v>
+      </c>
       <c r="K38" s="20" t="s">
         <v>12</v>
       </c>
@@ -2307,6 +2415,9 @@
       <c r="I39" s="1">
         <v>89212121</v>
       </c>
+      <c r="J39" s="1">
+        <v>4</v>
+      </c>
       <c r="K39" s="20" t="s">
         <v>12</v>
       </c>
@@ -2340,6 +2451,9 @@
       <c r="I40" s="1">
         <v>89212121</v>
       </c>
+      <c r="J40" s="1">
+        <v>4</v>
+      </c>
       <c r="K40" s="20" t="s">
         <v>12</v>
       </c>
@@ -2373,6 +2487,9 @@
       <c r="I41" s="1">
         <v>89212121</v>
       </c>
+      <c r="J41" s="1">
+        <v>4</v>
+      </c>
       <c r="K41" s="20" t="s">
         <v>12</v>
       </c>
@@ -2406,6 +2523,9 @@
       <c r="I42" s="1">
         <v>89212121</v>
       </c>
+      <c r="J42" s="1">
+        <v>4</v>
+      </c>
       <c r="K42" s="20" t="s">
         <v>12</v>
       </c>
@@ -2439,6 +2559,9 @@
       <c r="I43" s="1">
         <v>89212121</v>
       </c>
+      <c r="J43" s="1">
+        <v>4</v>
+      </c>
       <c r="K43" s="20" t="s">
         <v>12</v>
       </c>
@@ -2472,6 +2595,9 @@
       <c r="I44" s="1">
         <v>89212121</v>
       </c>
+      <c r="J44" s="1">
+        <v>4</v>
+      </c>
       <c r="K44" s="20" t="s">
         <v>12</v>
       </c>
@@ -2505,6 +2631,9 @@
       <c r="I45" s="1">
         <v>89212121</v>
       </c>
+      <c r="J45" s="1">
+        <v>4</v>
+      </c>
       <c r="K45" s="20" t="s">
         <v>12</v>
       </c>
@@ -2538,6 +2667,9 @@
       <c r="I46" s="1">
         <v>89212121</v>
       </c>
+      <c r="J46" s="1">
+        <v>4</v>
+      </c>
       <c r="K46" s="20" t="s">
         <v>12</v>
       </c>
@@ -2571,6 +2703,9 @@
       <c r="I47" s="1">
         <v>89212121</v>
       </c>
+      <c r="J47" s="1">
+        <v>4</v>
+      </c>
       <c r="K47" s="20" t="s">
         <v>12</v>
       </c>
@@ -2604,6 +2739,9 @@
       <c r="I48" s="1">
         <v>89212121</v>
       </c>
+      <c r="J48" s="1">
+        <v>4</v>
+      </c>
       <c r="K48" s="20" t="s">
         <v>12</v>
       </c>
@@ -2637,6 +2775,9 @@
       <c r="I49" s="1">
         <v>89212121</v>
       </c>
+      <c r="J49" s="1">
+        <v>4</v>
+      </c>
       <c r="K49" s="20" t="s">
         <v>12</v>
       </c>
@@ -2670,6 +2811,9 @@
       <c r="I50" s="1">
         <v>89212121</v>
       </c>
+      <c r="J50" s="1">
+        <v>4</v>
+      </c>
       <c r="K50" s="20" t="s">
         <v>12</v>
       </c>
@@ -2703,6 +2847,9 @@
       <c r="I51" s="1">
         <v>89212121</v>
       </c>
+      <c r="J51" s="1">
+        <v>4</v>
+      </c>
       <c r="K51" s="20" t="s">
         <v>12</v>
       </c>
@@ -2736,6 +2883,9 @@
       <c r="I52" s="1">
         <v>89212121</v>
       </c>
+      <c r="J52" s="1">
+        <v>4</v>
+      </c>
       <c r="K52" s="20" t="s">
         <v>12</v>
       </c>
@@ -2769,6 +2919,9 @@
       <c r="I53" s="1">
         <v>89212121</v>
       </c>
+      <c r="J53" s="1">
+        <v>4</v>
+      </c>
       <c r="K53" s="20" t="s">
         <v>12</v>
       </c>
@@ -2802,6 +2955,9 @@
       <c r="I54" s="1">
         <v>89212121</v>
       </c>
+      <c r="J54" s="1">
+        <v>4</v>
+      </c>
       <c r="K54" s="20" t="s">
         <v>12</v>
       </c>
@@ -2835,6 +2991,9 @@
       <c r="I55" s="1">
         <v>89212121</v>
       </c>
+      <c r="J55" s="1">
+        <v>4</v>
+      </c>
       <c r="K55" s="20" t="s">
         <v>12</v>
       </c>
@@ -2868,6 +3027,9 @@
       <c r="I56" s="1">
         <v>89212121</v>
       </c>
+      <c r="J56" s="1">
+        <v>4</v>
+      </c>
       <c r="K56" s="20" t="s">
         <v>12</v>
       </c>
@@ -2901,6 +3063,9 @@
       <c r="I57" s="1">
         <v>89212121</v>
       </c>
+      <c r="J57" s="1">
+        <v>4</v>
+      </c>
       <c r="K57" s="20" t="s">
         <v>12</v>
       </c>
@@ -2934,6 +3099,9 @@
       <c r="I58" s="1">
         <v>89212121</v>
       </c>
+      <c r="J58" s="1">
+        <v>4</v>
+      </c>
       <c r="K58" s="20" t="s">
         <v>12</v>
       </c>
@@ -2967,6 +3135,9 @@
       <c r="I59" s="1">
         <v>89212121</v>
       </c>
+      <c r="J59" s="1">
+        <v>4</v>
+      </c>
       <c r="K59" s="20" t="s">
         <v>12</v>
       </c>
@@ -3000,6 +3171,9 @@
       <c r="I60" s="1">
         <v>89212121</v>
       </c>
+      <c r="J60" s="1">
+        <v>4</v>
+      </c>
       <c r="K60" s="20" t="s">
         <v>12</v>
       </c>
@@ -3033,6 +3207,9 @@
       <c r="I61" s="1">
         <v>89212121</v>
       </c>
+      <c r="J61" s="1">
+        <v>4</v>
+      </c>
       <c r="K61" s="20" t="s">
         <v>12</v>
       </c>
@@ -3066,6 +3243,9 @@
       <c r="I62" s="1">
         <v>89212121</v>
       </c>
+      <c r="J62" s="1">
+        <v>4</v>
+      </c>
       <c r="K62" s="20" t="s">
         <v>12</v>
       </c>
@@ -3099,6 +3279,9 @@
       <c r="I63" s="1">
         <v>89212121</v>
       </c>
+      <c r="J63" s="1">
+        <v>4</v>
+      </c>
       <c r="K63" s="20" t="s">
         <v>12</v>
       </c>
@@ -3132,6 +3315,9 @@
       <c r="I64" s="1">
         <v>89212121</v>
       </c>
+      <c r="J64" s="1">
+        <v>4</v>
+      </c>
       <c r="K64" s="20" t="s">
         <v>12</v>
       </c>
@@ -3165,6 +3351,9 @@
       <c r="I65" s="1">
         <v>89212121</v>
       </c>
+      <c r="J65" s="1">
+        <v>4</v>
+      </c>
       <c r="K65" s="20" t="s">
         <v>12</v>
       </c>
@@ -3198,6 +3387,9 @@
       <c r="I66" s="1">
         <v>89212121</v>
       </c>
+      <c r="J66" s="1">
+        <v>4</v>
+      </c>
       <c r="K66" s="20" t="s">
         <v>12</v>
       </c>
@@ -3231,6 +3423,9 @@
       <c r="I67" s="1">
         <v>89212121</v>
       </c>
+      <c r="J67" s="1">
+        <v>4</v>
+      </c>
       <c r="K67" s="20" t="s">
         <v>12</v>
       </c>
@@ -3264,6 +3459,9 @@
       <c r="I68" s="1">
         <v>89212121</v>
       </c>
+      <c r="J68" s="1">
+        <v>4</v>
+      </c>
       <c r="K68" s="20" t="s">
         <v>12</v>
       </c>
@@ -3297,6 +3495,9 @@
       <c r="I69" s="1">
         <v>89212121</v>
       </c>
+      <c r="J69" s="1">
+        <v>4</v>
+      </c>
       <c r="K69" s="20" t="s">
         <v>12</v>
       </c>
@@ -3330,6 +3531,9 @@
       <c r="I70" s="1">
         <v>89212121</v>
       </c>
+      <c r="J70" s="1">
+        <v>4</v>
+      </c>
       <c r="K70" s="20" t="s">
         <v>12</v>
       </c>
@@ -3363,6 +3567,9 @@
       <c r="I71" s="1">
         <v>89212121</v>
       </c>
+      <c r="J71" s="1">
+        <v>4</v>
+      </c>
       <c r="K71" s="20" t="s">
         <v>12</v>
       </c>
@@ -3396,6 +3603,9 @@
       <c r="I72" s="1">
         <v>89212121</v>
       </c>
+      <c r="J72" s="1">
+        <v>4</v>
+      </c>
       <c r="K72" s="20" t="s">
         <v>12</v>
       </c>
@@ -3429,6 +3639,9 @@
       <c r="I73" s="1">
         <v>89212121</v>
       </c>
+      <c r="J73" s="1">
+        <v>4</v>
+      </c>
       <c r="K73" s="20" t="s">
         <v>12</v>
       </c>
@@ -3462,6 +3675,9 @@
       <c r="I74" s="1">
         <v>89212121</v>
       </c>
+      <c r="J74" s="1">
+        <v>4</v>
+      </c>
       <c r="K74" s="20" t="s">
         <v>12</v>
       </c>
@@ -3495,6 +3711,9 @@
       <c r="I75" s="1">
         <v>89212121</v>
       </c>
+      <c r="J75" s="1">
+        <v>4</v>
+      </c>
       <c r="K75" s="20" t="s">
         <v>12</v>
       </c>
@@ -3528,6 +3747,9 @@
       <c r="I76" s="1">
         <v>89212121</v>
       </c>
+      <c r="J76" s="1">
+        <v>4</v>
+      </c>
       <c r="K76" s="20" t="s">
         <v>12</v>
       </c>
@@ -3561,6 +3783,9 @@
       <c r="I77" s="1">
         <v>89212121</v>
       </c>
+      <c r="J77" s="1">
+        <v>4</v>
+      </c>
       <c r="K77" s="20" t="s">
         <v>12</v>
       </c>
@@ -3594,6 +3819,9 @@
       <c r="I78" s="1">
         <v>89212121</v>
       </c>
+      <c r="J78" s="1">
+        <v>4</v>
+      </c>
       <c r="K78" s="20" t="s">
         <v>12</v>
       </c>
@@ -3627,6 +3855,9 @@
       <c r="I79" s="1">
         <v>89212121</v>
       </c>
+      <c r="J79" s="1">
+        <v>4</v>
+      </c>
       <c r="K79" s="20" t="s">
         <v>12</v>
       </c>
@@ -3660,6 +3891,9 @@
       <c r="I80" s="1">
         <v>89212121</v>
       </c>
+      <c r="J80" s="1">
+        <v>4</v>
+      </c>
       <c r="K80" s="20" t="s">
         <v>12</v>
       </c>
@@ -3693,6 +3927,9 @@
       <c r="I81" s="1">
         <v>89212121</v>
       </c>
+      <c r="J81" s="1">
+        <v>4</v>
+      </c>
       <c r="K81" s="20" t="s">
         <v>12</v>
       </c>
@@ -3726,6 +3963,9 @@
       <c r="I82" s="1">
         <v>89212121</v>
       </c>
+      <c r="J82" s="1">
+        <v>4</v>
+      </c>
       <c r="K82" s="20" t="s">
         <v>12</v>
       </c>
@@ -3759,6 +3999,9 @@
       <c r="I83" s="1">
         <v>89212121</v>
       </c>
+      <c r="J83" s="1">
+        <v>4</v>
+      </c>
       <c r="K83" s="20" t="s">
         <v>12</v>
       </c>
@@ -3792,6 +4035,9 @@
       <c r="I84" s="1">
         <v>89212121</v>
       </c>
+      <c r="J84" s="1">
+        <v>4</v>
+      </c>
       <c r="K84" s="20" t="s">
         <v>12</v>
       </c>
@@ -3825,23 +4071,26 @@
       <c r="I85" s="1">
         <v>89212121</v>
       </c>
+      <c r="J85" s="1">
+        <v>4</v>
+      </c>
       <c r="K85" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L85" s="1"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="22"/>
-      <c r="B86" s="22"/>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
-      <c r="H86" s="22"/>
-      <c r="I86" s="22"/>
-      <c r="J86" s="22"/>
-      <c r="K86" s="22"/>
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
+      <c r="J86" s="21"/>
+      <c r="K86" s="21"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K85">

</xml_diff>